<commit_message>
4/28 update, current at 1.659
</commit_message>
<xml_diff>
--- a/PSPDASADCalculator.xlsx
+++ b/PSPDASADCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gonzagau-my.sharepoint.com/personal/stornquist_zagmail_gonzaga_edu/Documents/Junior year/Second Semester/Engineering Design/CMOS-Differential-Pair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{74CBE484-B1AF-45B1-9A96-B49E9F68C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{195995FB-A2C3-4949-ADE8-7E09B52E7F18}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{74CBE484-B1AF-45B1-9A96-B49E9F68C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0969B651-F5FA-4D5B-9879-29F0C2C3B0B9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F225980E-4B32-482E-82ED-67A38ECE05C3}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -191,8 +191,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +511,7 @@
   <dimension ref="C1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,24 +527,24 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <f>0.325</f>
         <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f>0.13</f>
         <v>0.13</v>
       </c>
@@ -553,45 +553,44 @@
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4">
-        <f>25</f>
-        <v>25</v>
+      <c r="D7" s="5">
+        <v>3.55</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <f>$D$7*$D$3</f>
-        <v>8.125</v>
+        <v>1.1537500000000001</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <f>$D$7*$D$3</f>
-        <v>8.125</v>
+        <v>1.1537500000000001</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <f>(2*D3)+D7</f>
-        <v>25.65</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6">
         <f>(2*D3)+D7</f>
-        <v>25.65</v>
+        <v>4.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5/6 update 20kHz BW(test1)
</commit_message>
<xml_diff>
--- a/PSPDASADCalculator.xlsx
+++ b/PSPDASADCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gonzagau-my.sharepoint.com/personal/stornquist_zagmail_gonzaga_edu/Documents/Junior year/Second Semester/Engineering Design/CMOS-Differential-Pair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{74CBE484-B1AF-45B1-9A96-B49E9F68C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FA1F44AF-DB1F-42EB-ACDA-ED1879FB4944}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{74CBE484-B1AF-45B1-9A96-B49E9F68C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FE52FDEF-56E1-4A6E-A6E5-201CBE63C868}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F225980E-4B32-482E-82ED-67A38ECE05C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F225980E-4B32-482E-82ED-67A38ECE05C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,11 +677,12 @@
   <dimension ref="C1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -819,8 +820,8 @@
         <v>0</v>
       </c>
       <c r="D6" s="5">
-        <f>0.13</f>
-        <v>0.13</v>
+        <f>0.44</f>
+        <v>0.44</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
@@ -836,7 +837,8 @@
         <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>3.55</v>
+        <f>1000</f>
+        <v>1000</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>12</v>
@@ -856,7 +858,7 @@
       </c>
       <c r="D8" s="5">
         <f>$D$7*$D$3</f>
-        <v>1.1537500000000001</v>
+        <v>325</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -879,7 +881,7 @@
       </c>
       <c r="D9" s="5">
         <f>$D$7*$D$3</f>
-        <v>1.1537500000000001</v>
+        <v>325</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
@@ -892,8 +894,8 @@
         <v>4</v>
       </c>
       <c r="D10" s="5">
-        <f>(2*D3)+D7</f>
-        <v>4.2</v>
+        <f>(2*D3)+(2*D7)</f>
+        <v>2000.65</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>19</v>
@@ -905,8 +907,8 @@
         <v>5</v>
       </c>
       <c r="D11" s="6">
-        <f>(2*D3)+D7</f>
-        <v>4.2</v>
+        <f>(2*D3)+(2*D7)</f>
+        <v>2000.65</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
ACTUALLY finalized design 5/7, ~30 dB DC gain, 175 kHz 0 dB bandwidth
</commit_message>
<xml_diff>
--- a/PSPDASADCalculator.xlsx
+++ b/PSPDASADCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholas/Documents/CMOS-Differential-Pair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39525AD0-C42A-1540-90B9-422547508CB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F808B-10E7-F34D-A803-9E08167BB3E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F225980E-4B32-482E-82ED-67A38ECE05C3}"/>
   </bookViews>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="5">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>9.1524999999999999</v>
+        <v>9.6909299999999998</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>12</v>
@@ -856,7 +856,7 @@
       </c>
       <c r="D8" s="5">
         <f>$D$7*$D$3</f>
-        <v>2.9745625000000002</v>
+        <v>3.1495522500000002</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -879,7 +879,7 @@
       </c>
       <c r="D9" s="5">
         <f>$D$7*$D$3</f>
-        <v>2.9745625000000002</v>
+        <v>3.1495522500000002</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
@@ -893,7 +893,7 @@
       </c>
       <c r="D10" s="5">
         <f>(2*D3)+(2*D7)</f>
-        <v>18.954999999999998</v>
+        <v>20.031859999999998</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>19</v>
@@ -906,7 +906,7 @@
       </c>
       <c r="D11" s="6">
         <f>(2*D3)+(2*D7)</f>
-        <v>18.954999999999998</v>
+        <v>20.031859999999998</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>20</v>

</xml_diff>